<commit_message>
continuing update on prep columns
</commit_message>
<xml_diff>
--- a/old_database/crypto/s1cDNASample/s1cDNASample_0629_0618.xlsx
+++ b/old_database/crypto/s1cDNASample/s1cDNASample_0629_0618.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">s1cDNASampleNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">s1cDNAProtocol </t>
+    <t xml:space="preserve">s1cDNAProtocol</t>
   </si>
   <si>
     <t xml:space="preserve">10.07.11</t>
@@ -175,7 +175,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G25"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>